<commit_message>
Update descriptions in model
</commit_message>
<xml_diff>
--- a/BC Data Model Outline.xlsx
+++ b/BC Data Model Outline.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Linda\Documents\CDISC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\cdisc-org\COSMoS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2EB5F9A5-B9F4-42AA-A825-2150AEBBFEC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A558C6E-4E5B-455F-A2A0-9569685656F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{FA29263D-F7AA-4D0C-AE9B-6B008D3B18BE}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{FA29263D-F7AA-4D0C-AE9B-6B008D3B18BE}"/>
   </bookViews>
   <sheets>
     <sheet name="BC Data Model" sheetId="8" r:id="rId1"/>
@@ -1349,30 +1349,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6575D01-805D-0E4D-89C4-3AB8EBDBFBB8}">
   <dimension ref="A1:R71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="13.17578125" style="2" customWidth="1"/>
-    <col min="3" max="4" width="15.8203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="20.17578125" style="2" customWidth="1"/>
-    <col min="6" max="7" width="17.703125" style="9" customWidth="1"/>
-    <col min="8" max="8" width="23.703125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="16.3515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.05859375" style="3" customWidth="1"/>
-    <col min="11" max="11" width="16.3515625" style="3" customWidth="1"/>
-    <col min="12" max="12" width="22.29296875" style="2" customWidth="1"/>
-    <col min="13" max="13" width="17.52734375" style="2" customWidth="1"/>
+    <col min="1" max="2" width="13.140625" style="2" customWidth="1"/>
+    <col min="3" max="4" width="15.85546875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" style="2" customWidth="1"/>
+    <col min="6" max="7" width="17.7109375" style="9" customWidth="1"/>
+    <col min="8" max="8" width="23.7109375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30" style="3" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" style="3" customWidth="1"/>
+    <col min="12" max="12" width="22.28515625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="17.5703125" style="2" customWidth="1"/>
     <col min="14" max="15" width="17" style="2" customWidth="1"/>
-    <col min="16" max="16" width="17.17578125" style="2" customWidth="1"/>
-    <col min="17" max="17" width="17.3515625" style="2" customWidth="1"/>
-    <col min="18" max="18" width="16.87890625" style="3" customWidth="1"/>
+    <col min="16" max="16" width="17.140625" style="2" customWidth="1"/>
+    <col min="17" max="17" width="17.28515625" style="2" customWidth="1"/>
+    <col min="18" max="18" width="16.85546875" style="3" customWidth="1"/>
     <col min="19" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:18" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
         <v>156</v>
       </c>
@@ -1425,7 +1425,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:18" s="46" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:18" s="46" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
         <v>16</v>
       </c>
@@ -1481,7 +1481,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="3" spans="1:18" s="23" customFormat="1" ht="100.35" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:18" s="23" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
         <v>3</v>
       </c>
@@ -1534,7 +1534,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="4" spans="1:18" s="22" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:18" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="53" t="s">
         <v>4</v>
       </c>
@@ -1590,7 +1590,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:18" s="22" customFormat="1" ht="15.5" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:18" s="22" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="53" t="s">
         <v>5</v>
       </c>
@@ -1646,7 +1646,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:18" s="22" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:18" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="53" t="s">
         <v>6</v>
       </c>
@@ -1702,7 +1702,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:18" s="22" customFormat="1" ht="71.7" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:18" s="22" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="53" t="s">
         <v>7</v>
       </c>
@@ -1715,7 +1715,7 @@
       </c>
       <c r="R7" s="23"/>
     </row>
-    <row r="8" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>0</v>
       </c>
@@ -1732,7 +1732,7 @@
       <c r="Q8" s="9"/>
       <c r="R8" s="14"/>
     </row>
-    <row r="9" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1746,7 +1746,7 @@
       <c r="Q9" s="9"/>
       <c r="R9" s="9"/>
     </row>
-    <row r="11" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
       <c r="B11" s="9"/>
       <c r="C11" s="2"/>
@@ -1760,7 +1760,7 @@
       <c r="Q11" s="9"/>
       <c r="R11" s="14"/>
     </row>
-    <row r="12" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
       <c r="B12" s="9"/>
       <c r="C12" s="2"/>
@@ -1774,7 +1774,7 @@
       <c r="Q12" s="9"/>
       <c r="R12" s="14"/>
     </row>
-    <row r="13" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
       <c r="B13" s="9"/>
       <c r="C13" s="2"/>
@@ -1788,7 +1788,7 @@
       <c r="Q13" s="9"/>
       <c r="R13" s="14"/>
     </row>
-    <row r="14" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
       <c r="B14" s="9"/>
       <c r="C14" s="2"/>
@@ -1802,7 +1802,7 @@
       <c r="Q14" s="9"/>
       <c r="R14" s="9"/>
     </row>
-    <row r="15" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
       <c r="B15" s="9"/>
       <c r="C15" s="2"/>
@@ -1816,7 +1816,7 @@
       <c r="Q15" s="9"/>
       <c r="R15" s="9"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
       <c r="B16" s="9"/>
       <c r="H16" s="9"/>
@@ -1824,7 +1824,7 @@
       <c r="J16" s="14"/>
       <c r="K16" s="14"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
       <c r="B17" s="9"/>
       <c r="H17" s="9"/>
@@ -1832,7 +1832,7 @@
       <c r="J17" s="14"/>
       <c r="K17" s="14"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
       <c r="B18" s="9"/>
       <c r="I18" s="14"/>
@@ -1844,7 +1844,7 @@
       <c r="Q18" s="9"/>
       <c r="R18" s="9"/>
     </row>
-    <row r="19" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
       <c r="B19" s="9"/>
       <c r="C19" s="2"/>
@@ -1861,7 +1861,7 @@
       <c r="Q19" s="9"/>
       <c r="R19" s="9"/>
     </row>
-    <row r="20" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
       <c r="B20" s="9"/>
       <c r="C20" s="2"/>
@@ -1878,7 +1878,7 @@
       <c r="Q20" s="9"/>
       <c r="R20" s="9"/>
     </row>
-    <row r="21" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
       <c r="B21" s="9"/>
       <c r="C21" s="2"/>
@@ -1895,7 +1895,7 @@
       <c r="Q21" s="9"/>
       <c r="R21" s="9"/>
     </row>
-    <row r="22" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>
       <c r="B22" s="9"/>
       <c r="C22" s="2"/>
@@ -1913,11 +1913,11 @@
       <c r="Q22" s="9"/>
       <c r="R22" s="9"/>
     </row>
-    <row r="23" spans="1:18" ht="15.5" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:18" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
       <c r="B23" s="9"/>
     </row>
-    <row r="24" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9"/>
       <c r="B24" s="9"/>
       <c r="C24" s="2"/>
@@ -1931,7 +1931,7 @@
       <c r="Q24" s="9"/>
       <c r="R24" s="14"/>
     </row>
-    <row r="25" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -1945,7 +1945,7 @@
       <c r="Q25" s="9"/>
       <c r="R25" s="14"/>
     </row>
-    <row r="26" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -1959,7 +1959,7 @@
       <c r="Q26" s="9"/>
       <c r="R26" s="14"/>
     </row>
-    <row r="27" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -1973,69 +1973,69 @@
       <c r="Q27" s="9"/>
       <c r="R27" s="9"/>
     </row>
-    <row r="28" spans="1:18" ht="30.45" customHeight="1" x14ac:dyDescent="0.5"/>
-    <row r="29" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:18" ht="30.4" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="I29" s="14"/>
       <c r="J29" s="14"/>
       <c r="K29" s="14"/>
     </row>
-    <row r="30" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
     </row>
-    <row r="31" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
     </row>
-    <row r="32" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="I32" s="18"/>
       <c r="J32" s="18"/>
       <c r="K32" s="18"/>
     </row>
-    <row r="33" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
     </row>
-    <row r="34" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="I34" s="14"/>
       <c r="J34" s="14"/>
       <c r="K34" s="14"/>
     </row>
-    <row r="35" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
     </row>
-    <row r="36" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
     </row>
-    <row r="37" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="N37" s="8"/>
       <c r="O37" s="8"/>
     </row>
-    <row r="38" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
     </row>
-    <row r="39" spans="1:18" s="9" customFormat="1" ht="28.45" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:18" s="9" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="I39" s="14"/>
       <c r="J39" s="14"/>
       <c r="K39" s="14"/>
     </row>
-    <row r="40" spans="1:18" ht="15.5" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:18" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E40" s="9"/>
     </row>
-    <row r="41" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -2049,7 +2049,7 @@
       <c r="Q41" s="9"/>
       <c r="R41" s="14"/>
     </row>
-    <row r="42" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -2063,7 +2063,7 @@
       <c r="Q42" s="9"/>
       <c r="R42" s="14"/>
     </row>
-    <row r="43" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -2077,7 +2077,7 @@
       <c r="Q43" s="9"/>
       <c r="R43" s="14"/>
     </row>
-    <row r="44" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -2091,10 +2091,10 @@
       <c r="Q44" s="9"/>
       <c r="R44" s="9"/>
     </row>
-    <row r="45" spans="1:18" ht="15.5" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:18" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E45" s="9"/>
     </row>
-    <row r="46" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -2108,7 +2108,7 @@
       <c r="Q46" s="9"/>
       <c r="R46" s="14"/>
     </row>
-    <row r="47" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -2122,7 +2122,7 @@
       <c r="Q47" s="9"/>
       <c r="R47" s="14"/>
     </row>
-    <row r="48" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -2136,7 +2136,7 @@
       <c r="Q48" s="9"/>
       <c r="R48" s="14"/>
     </row>
-    <row r="49" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="49" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -2150,7 +2150,7 @@
       <c r="Q49" s="9"/>
       <c r="R49" s="9"/>
     </row>
-    <row r="50" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="50" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -2167,12 +2167,12 @@
       <c r="Q50" s="9"/>
       <c r="R50" s="9"/>
     </row>
-    <row r="51" spans="1:18" ht="15.5" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:18" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E51" s="9"/>
       <c r="L51" s="9"/>
       <c r="M51" s="9"/>
     </row>
-    <row r="52" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
@@ -2187,7 +2187,7 @@
       <c r="Q52" s="9"/>
       <c r="R52" s="14"/>
     </row>
-    <row r="53" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -2201,7 +2201,7 @@
       <c r="Q53" s="9"/>
       <c r="R53" s="14"/>
     </row>
-    <row r="54" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="54" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -2215,7 +2215,7 @@
       <c r="Q54" s="9"/>
       <c r="R54" s="14"/>
     </row>
-    <row r="55" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -2229,12 +2229,12 @@
       <c r="Q55" s="9"/>
       <c r="R55" s="9"/>
     </row>
-    <row r="56" spans="1:18" ht="15.5" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="56" spans="1:18" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E56" s="9"/>
       <c r="L56" s="9"/>
       <c r="M56" s="9"/>
     </row>
-    <row r="57" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="57" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -2249,7 +2249,7 @@
       <c r="Q57" s="9"/>
       <c r="R57" s="14"/>
     </row>
-    <row r="58" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="58" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
@@ -2263,7 +2263,7 @@
       <c r="Q58" s="9"/>
       <c r="R58" s="14"/>
     </row>
-    <row r="59" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="59" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
@@ -2277,7 +2277,7 @@
       <c r="Q59" s="9"/>
       <c r="R59" s="14"/>
     </row>
-    <row r="60" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="60" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
@@ -2291,7 +2291,7 @@
       <c r="Q60" s="9"/>
       <c r="R60" s="9"/>
     </row>
-    <row r="61" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="61" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -2308,7 +2308,7 @@
       <c r="Q61" s="9"/>
       <c r="R61" s="9"/>
     </row>
-    <row r="62" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="62" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
@@ -2328,7 +2328,7 @@
       <c r="Q62" s="9"/>
       <c r="R62" s="9"/>
     </row>
-    <row r="63" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="63" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
@@ -2346,7 +2346,7 @@
       <c r="Q63" s="9"/>
       <c r="R63" s="14"/>
     </row>
-    <row r="64" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="64" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
@@ -2364,7 +2364,7 @@
       <c r="Q64" s="9"/>
       <c r="R64" s="14"/>
     </row>
-    <row r="65" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="65" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
@@ -2382,7 +2382,7 @@
       <c r="Q65" s="9"/>
       <c r="R65" s="14"/>
     </row>
-    <row r="66" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="66" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
@@ -2400,11 +2400,11 @@
       <c r="Q66" s="9"/>
       <c r="R66" s="9"/>
     </row>
-    <row r="67" spans="1:18" ht="15.5" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="67" spans="1:18" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L67" s="9"/>
       <c r="M67" s="9"/>
     </row>
-    <row r="68" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="68" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
@@ -2419,7 +2419,7 @@
       <c r="Q68" s="9"/>
       <c r="R68" s="14"/>
     </row>
-    <row r="69" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="69" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
@@ -2433,7 +2433,7 @@
       <c r="Q69" s="9"/>
       <c r="R69" s="14"/>
     </row>
-    <row r="70" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="70" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
@@ -2447,7 +2447,7 @@
       <c r="Q70" s="9"/>
       <c r="R70" s="14"/>
     </row>
-    <row r="71" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="71" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
@@ -2476,43 +2476,43 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.87890625" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.17578125" style="27" customWidth="1"/>
-    <col min="2" max="2" width="20.17578125" customWidth="1"/>
-    <col min="3" max="3" width="18.17578125" customWidth="1"/>
-    <col min="4" max="4" width="17.05859375" customWidth="1"/>
-    <col min="5" max="6" width="20.17578125" customWidth="1"/>
-    <col min="7" max="8" width="18.17578125" customWidth="1"/>
-    <col min="9" max="10" width="25.703125" customWidth="1"/>
-    <col min="11" max="11" width="13.87890625" customWidth="1"/>
-    <col min="12" max="12" width="13.29296875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.29296875" customWidth="1"/>
-    <col min="14" max="14" width="13.87890625" customWidth="1"/>
-    <col min="15" max="15" width="15.8203125" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" style="27" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
+    <col min="5" max="6" width="20.140625" customWidth="1"/>
+    <col min="7" max="8" width="18.140625" customWidth="1"/>
+    <col min="9" max="10" width="25.7109375" customWidth="1"/>
+    <col min="11" max="11" width="13.85546875" customWidth="1"/>
+    <col min="12" max="12" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.28515625" customWidth="1"/>
+    <col min="14" max="14" width="13.85546875" customWidth="1"/>
+    <col min="15" max="15" width="15.85546875" customWidth="1"/>
     <col min="16" max="16" width="18" customWidth="1"/>
-    <col min="17" max="17" width="16.8203125" customWidth="1"/>
-    <col min="18" max="18" width="16.52734375" customWidth="1"/>
-    <col min="19" max="19" width="12.46875" customWidth="1"/>
-    <col min="20" max="20" width="18.46875" customWidth="1"/>
-    <col min="21" max="21" width="35.8203125" style="11" customWidth="1"/>
-    <col min="22" max="22" width="25.703125" style="11" customWidth="1"/>
-    <col min="23" max="23" width="18.52734375" customWidth="1"/>
-    <col min="24" max="24" width="15.703125" customWidth="1"/>
-    <col min="25" max="25" width="14.05859375" customWidth="1"/>
-    <col min="26" max="27" width="16.703125" customWidth="1"/>
-    <col min="28" max="28" width="19.05859375" customWidth="1"/>
-    <col min="29" max="29" width="21.05859375" customWidth="1"/>
-    <col min="30" max="30" width="16.52734375" customWidth="1"/>
+    <col min="17" max="17" width="16.85546875" customWidth="1"/>
+    <col min="18" max="18" width="16.5703125" customWidth="1"/>
+    <col min="19" max="19" width="12.42578125" customWidth="1"/>
+    <col min="20" max="20" width="18.42578125" customWidth="1"/>
+    <col min="21" max="21" width="35.85546875" style="11" customWidth="1"/>
+    <col min="22" max="22" width="25.7109375" style="11" customWidth="1"/>
+    <col min="23" max="23" width="18.5703125" customWidth="1"/>
+    <col min="24" max="24" width="15.7109375" customWidth="1"/>
+    <col min="25" max="25" width="14" customWidth="1"/>
+    <col min="26" max="27" width="16.7109375" customWidth="1"/>
+    <col min="28" max="28" width="19" customWidth="1"/>
+    <col min="29" max="29" width="21" customWidth="1"/>
+    <col min="30" max="30" width="16.5703125" customWidth="1"/>
     <col min="31" max="31" width="15" customWidth="1"/>
-    <col min="32" max="32" width="26.52734375" customWidth="1"/>
-    <col min="33" max="33" width="20.17578125" customWidth="1"/>
-    <col min="34" max="35" width="13.05859375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="26.5703125" customWidth="1"/>
+    <col min="33" max="33" width="20.140625" customWidth="1"/>
+    <col min="34" max="35" width="13" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="14" customWidth="1"/>
-    <col min="37" max="41" width="13.703125" customWidth="1"/>
+    <col min="37" max="41" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" s="1" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:41" s="1" customFormat="1" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>46</v>
       </c>
@@ -2637,7 +2637,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:41" s="22" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:41" s="22" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
         <v>22</v>
       </c>
@@ -2762,7 +2762,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="3" spans="1:41" s="55" customFormat="1" ht="86" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:41" s="55" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" s="38" t="s">
         <v>3</v>
       </c>
@@ -2875,7 +2875,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:41" s="30" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:41" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="30" t="s">
         <v>4</v>
       </c>
@@ -3000,7 +3000,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:41" s="30" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:41" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="30" t="s">
         <v>5</v>
       </c>
@@ -3125,7 +3125,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:41" s="30" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:41" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="30" t="s">
         <v>6</v>
       </c>
@@ -3250,7 +3250,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:41" s="30" customFormat="1" ht="215" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:41" s="30" customFormat="1" ht="240" x14ac:dyDescent="0.25">
       <c r="A7" s="30" t="s">
         <v>7</v>
       </c>
@@ -3285,7 +3285,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="8" spans="1:41" s="15" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:41" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="27"/>
       <c r="B8" s="19"/>
       <c r="E8" s="19"/>
@@ -3294,7 +3294,7 @@
       <c r="J8" s="19"/>
       <c r="V8" s="21"/>
     </row>
-    <row r="9" spans="1:41" s="15" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:41" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="27"/>
       <c r="B9" s="19"/>
       <c r="E9" s="19"/>
@@ -3303,84 +3303,84 @@
       <c r="J9" s="19"/>
       <c r="V9" s="21"/>
     </row>
-    <row r="10" spans="1:41" s="6" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:41" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="27"/>
       <c r="U10" s="16"/>
       <c r="V10" s="20"/>
       <c r="W10" s="16"/>
     </row>
-    <row r="11" spans="1:41" s="6" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:41" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="28"/>
       <c r="U11" s="16"/>
       <c r="V11" s="20"/>
     </row>
-    <row r="12" spans="1:41" s="6" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:41" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="28"/>
       <c r="U12" s="16"/>
       <c r="V12" s="20"/>
     </row>
-    <row r="13" spans="1:41" s="6" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:41" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="28"/>
       <c r="U13" s="16"/>
       <c r="V13" s="20"/>
     </row>
-    <row r="14" spans="1:41" s="6" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:41" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="28"/>
       <c r="U14" s="16"/>
       <c r="V14" s="16"/>
     </row>
-    <row r="15" spans="1:41" s="6" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:41" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="28"/>
       <c r="U15" s="16"/>
       <c r="V15" s="16"/>
     </row>
-    <row r="16" spans="1:41" s="6" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:41" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="28"/>
       <c r="U16" s="16"/>
       <c r="V16" s="16"/>
     </row>
-    <row r="17" spans="1:23" s="15" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:23" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="28"/>
       <c r="V17" s="21"/>
       <c r="W17" s="17"/>
     </row>
-    <row r="18" spans="1:23" s="15" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:23" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="28"/>
       <c r="U18" s="17"/>
       <c r="V18" s="21"/>
     </row>
-    <row r="19" spans="1:23" s="15" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:23" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="28"/>
       <c r="U19" s="17"/>
       <c r="V19" s="21"/>
     </row>
-    <row r="20" spans="1:23" s="15" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:23" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="28"/>
       <c r="U20" s="17"/>
       <c r="V20" s="21"/>
     </row>
-    <row r="21" spans="1:23" s="15" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:23" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="28"/>
       <c r="U21" s="17"/>
       <c r="V21" s="17"/>
     </row>
-    <row r="22" spans="1:23" s="15" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:23" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="28"/>
       <c r="U22" s="17"/>
       <c r="V22" s="17"/>
     </row>
-    <row r="23" spans="1:23" s="15" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:23" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="28"/>
       <c r="U23" s="17"/>
       <c r="V23" s="17"/>
     </row>
-    <row r="24" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="28"/>
       <c r="U24" s="16"/>
       <c r="V24" s="20"/>
       <c r="W24" s="16"/>
     </row>
-    <row r="25" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="27"/>
       <c r="T25" s="6" t="s">
         <v>55</v>
@@ -3388,150 +3388,150 @@
       <c r="U25" s="16"/>
       <c r="V25" s="20"/>
     </row>
-    <row r="26" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="27"/>
       <c r="U26" s="16"/>
       <c r="V26" s="20"/>
     </row>
-    <row r="27" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="27"/>
       <c r="U27" s="16"/>
       <c r="V27" s="20"/>
     </row>
-    <row r="28" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="27"/>
       <c r="U28" s="16"/>
       <c r="V28" s="16"/>
     </row>
-    <row r="29" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="27"/>
       <c r="U29" s="16"/>
       <c r="V29" s="16"/>
     </row>
-    <row r="30" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="27"/>
       <c r="U30" s="16"/>
       <c r="V30" s="16"/>
     </row>
-    <row r="31" spans="1:23" s="15" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:23" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="27"/>
       <c r="V31" s="21"/>
     </row>
-    <row r="32" spans="1:23" s="15" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:23" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="27"/>
       <c r="V32" s="21"/>
     </row>
-    <row r="33" spans="1:23" s="15" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:23" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="27"/>
       <c r="V33" s="21"/>
     </row>
-    <row r="34" spans="1:23" s="15" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:23" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="27"/>
       <c r="V34" s="21"/>
     </row>
-    <row r="35" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="27"/>
       <c r="U35" s="16"/>
       <c r="V35" s="20"/>
       <c r="W35" s="16"/>
     </row>
-    <row r="36" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="27"/>
       <c r="U36" s="16"/>
       <c r="V36" s="20"/>
     </row>
-    <row r="37" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="27"/>
       <c r="U37" s="16"/>
       <c r="V37" s="20"/>
     </row>
-    <row r="38" spans="1:23" s="15" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:23" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="27"/>
       <c r="V38" s="21"/>
       <c r="W38" s="17"/>
     </row>
-    <row r="39" spans="1:23" s="15" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:23" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="27"/>
       <c r="U39" s="17"/>
       <c r="V39" s="21"/>
     </row>
-    <row r="40" spans="1:23" s="15" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:23" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="27"/>
       <c r="U40" s="17"/>
       <c r="V40" s="21"/>
     </row>
-    <row r="41" spans="1:23" s="15" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:23" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="27"/>
       <c r="U41" s="17"/>
       <c r="V41" s="21"/>
     </row>
-    <row r="42" spans="1:23" s="15" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:23" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="27"/>
       <c r="U42" s="17"/>
       <c r="V42" s="17"/>
     </row>
-    <row r="43" spans="1:23" s="15" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:23" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="27"/>
       <c r="U43" s="17"/>
       <c r="V43" s="17"/>
     </row>
-    <row r="44" spans="1:23" s="15" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:23" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="27"/>
       <c r="U44" s="17"/>
       <c r="V44" s="17"/>
     </row>
-    <row r="45" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="27"/>
       <c r="V45" s="20"/>
       <c r="W45" s="16"/>
     </row>
-    <row r="46" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="27"/>
       <c r="U46" s="16"/>
       <c r="V46" s="20"/>
     </row>
-    <row r="47" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="27"/>
       <c r="U47" s="16"/>
       <c r="V47" s="20"/>
     </row>
-    <row r="48" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="27"/>
       <c r="U48" s="16"/>
       <c r="V48" s="20"/>
     </row>
-    <row r="49" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="49" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="27"/>
       <c r="U49" s="16"/>
       <c r="V49" s="16"/>
     </row>
-    <row r="50" spans="1:23" s="15" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="50" spans="1:23" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="27"/>
       <c r="V50" s="21"/>
       <c r="W50" s="17"/>
     </row>
-    <row r="51" spans="1:23" s="15" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:23" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="27"/>
       <c r="U51" s="17"/>
       <c r="V51" s="21"/>
     </row>
-    <row r="52" spans="1:23" s="15" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:23" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="27"/>
       <c r="P52" s="6"/>
       <c r="U52" s="17"/>
       <c r="V52" s="21"/>
     </row>
-    <row r="53" spans="1:23" s="15" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:23" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="27"/>
       <c r="U53" s="17"/>
       <c r="V53" s="21"/>
     </row>
-    <row r="54" spans="1:23" s="15" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="54" spans="1:23" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="27"/>
       <c r="U54" s="17"/>
       <c r="V54" s="17"/>
     </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
       <c r="P55" s="15"/>
     </row>
   </sheetData>
@@ -3549,34 +3549,34 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.87890625" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.05859375" customWidth="1"/>
-    <col min="2" max="3" width="16.52734375" customWidth="1"/>
-    <col min="4" max="4" width="18.87890625" customWidth="1"/>
-    <col min="5" max="5" width="20.05859375" customWidth="1"/>
-    <col min="6" max="6" width="16.05859375" customWidth="1"/>
-    <col min="7" max="7" width="15.3515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="19.87890625" customWidth="1"/>
-    <col min="10" max="10" width="35.05859375" customWidth="1"/>
-    <col min="11" max="12" width="24.3515625" customWidth="1"/>
-    <col min="13" max="13" width="26.46875" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="24.3515625" customWidth="1"/>
-    <col min="16" max="16" width="15.52734375" customWidth="1"/>
-    <col min="17" max="17" width="13.8203125" customWidth="1"/>
-    <col min="18" max="18" width="17.3515625" customWidth="1"/>
-    <col min="19" max="19" width="13.05859375" style="11" customWidth="1"/>
-    <col min="20" max="20" width="19.703125" style="11" customWidth="1"/>
-    <col min="21" max="21" width="13.64453125" customWidth="1"/>
-    <col min="22" max="23" width="13.05859375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="2" max="3" width="16.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" customWidth="1"/>
+    <col min="5" max="5" width="20" customWidth="1"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="19.85546875" customWidth="1"/>
+    <col min="10" max="10" width="35" customWidth="1"/>
+    <col min="11" max="12" width="24.28515625" customWidth="1"/>
+    <col min="13" max="13" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="24.28515625" customWidth="1"/>
+    <col min="16" max="16" width="15.5703125" customWidth="1"/>
+    <col min="17" max="17" width="13.85546875" customWidth="1"/>
+    <col min="18" max="18" width="17.28515625" customWidth="1"/>
+    <col min="19" max="19" width="13" style="11" customWidth="1"/>
+    <col min="20" max="20" width="19.7109375" style="11" customWidth="1"/>
+    <col min="21" max="21" width="13.7109375" customWidth="1"/>
+    <col min="22" max="23" width="13" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="14" customWidth="1"/>
-    <col min="25" max="25" width="13.703125" customWidth="1"/>
+    <col min="25" max="25" width="13.7109375" customWidth="1"/>
     <col min="26" max="26" width="13" customWidth="1"/>
-    <col min="27" max="29" width="13.703125" customWidth="1"/>
-    <col min="30" max="30" width="16.87890625" customWidth="1"/>
+    <col min="27" max="29" width="13.7109375" customWidth="1"/>
+    <col min="30" max="30" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="1" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:30" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
         <v>19</v>
       </c>
@@ -3668,7 +3668,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:30" s="33" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:30" s="33" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
         <v>22</v>
       </c>
@@ -3757,7 +3757,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="3" spans="1:30" s="57" customFormat="1" ht="71.7" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:30" s="57" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="57" t="s">
         <v>3</v>
       </c>
@@ -3834,7 +3834,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
         <v>4</v>
       </c>
@@ -3923,7 +3923,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
         <v>5</v>
       </c>
@@ -4009,7 +4009,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
         <v>6</v>
       </c>
@@ -4095,7 +4095,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:30" s="33" customFormat="1" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:30" s="33" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
         <v>7</v>
       </c>
@@ -4128,7 +4128,7 @@
       <c r="AB7" s="26"/>
       <c r="AC7" s="26"/>
     </row>
-    <row r="8" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F8" s="16"/>
       <c r="G8" s="29"/>
       <c r="J8" s="16"/>
@@ -4146,7 +4146,7 @@
       <c r="AB8" s="15"/>
       <c r="AC8" s="15"/>
     </row>
-    <row r="9" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F9" s="16"/>
       <c r="G9" s="29"/>
       <c r="J9" s="16"/>
@@ -4164,7 +4164,7 @@
       <c r="AB9" s="15"/>
       <c r="AC9" s="15"/>
     </row>
-    <row r="10" spans="1:30" s="15" customFormat="1" ht="43.45" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:30" s="15" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F10" s="17"/>
       <c r="G10" s="17"/>
       <c r="J10" s="17"/>
@@ -4179,7 +4179,7 @@
       <c r="AB10" s="6"/>
       <c r="AC10" s="6"/>
     </row>
-    <row r="11" spans="1:30" s="15" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:30" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F11" s="17"/>
       <c r="G11" s="17"/>
       <c r="J11" s="17"/>
@@ -4194,77 +4194,77 @@
       <c r="AB11" s="6"/>
       <c r="AC11" s="6"/>
     </row>
-    <row r="12" spans="1:30" s="6" customFormat="1" ht="43.45" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:30" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
       <c r="J12" s="16"/>
       <c r="S12" s="16"/>
       <c r="T12" s="16"/>
     </row>
-    <row r="13" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
       <c r="J13" s="16"/>
       <c r="S13" s="16"/>
       <c r="T13" s="16"/>
     </row>
-    <row r="14" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
       <c r="J14" s="16"/>
       <c r="S14" s="16"/>
       <c r="T14" s="16"/>
     </row>
-    <row r="15" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F15" s="16"/>
       <c r="G15" s="16"/>
       <c r="J15" s="16"/>
       <c r="S15" s="16"/>
       <c r="T15" s="16"/>
     </row>
-    <row r="16" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F16" s="16"/>
       <c r="G16" s="16"/>
       <c r="J16" s="16"/>
       <c r="S16" s="16"/>
       <c r="T16" s="16"/>
     </row>
-    <row r="17" spans="6:29" s="15" customFormat="1" ht="43.45" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="17" spans="6:29" s="15" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F17" s="17"/>
       <c r="G17" s="17"/>
       <c r="J17" s="17"/>
       <c r="S17" s="17"/>
       <c r="T17" s="17"/>
     </row>
-    <row r="18" spans="6:29" s="15" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="18" spans="6:29" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F18" s="17"/>
       <c r="G18" s="17"/>
       <c r="J18" s="17"/>
       <c r="S18" s="17"/>
       <c r="T18" s="17"/>
     </row>
-    <row r="19" spans="6:29" s="15" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="19" spans="6:29" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F19" s="17"/>
       <c r="G19" s="17"/>
       <c r="J19" s="17"/>
       <c r="S19" s="17"/>
       <c r="T19" s="17"/>
     </row>
-    <row r="20" spans="6:29" s="15" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="20" spans="6:29" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
       <c r="J20" s="17"/>
       <c r="S20" s="17"/>
       <c r="T20" s="17"/>
     </row>
-    <row r="21" spans="6:29" s="15" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="21" spans="6:29" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F21" s="17"/>
       <c r="G21" s="17"/>
       <c r="J21" s="17"/>
       <c r="S21" s="17"/>
       <c r="T21" s="17"/>
     </row>
-    <row r="22" spans="6:29" s="6" customFormat="1" ht="43.45" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="22" spans="6:29" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F22" s="16"/>
       <c r="G22" s="16"/>
       <c r="J22" s="16"/>
@@ -4279,7 +4279,7 @@
       <c r="AB22" s="15"/>
       <c r="AC22" s="15"/>
     </row>
-    <row r="23" spans="6:29" s="6" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="23" spans="6:29" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F23" s="16"/>
       <c r="G23" s="16"/>
       <c r="J23" s="16"/>
@@ -4294,28 +4294,28 @@
       <c r="AB23" s="15"/>
       <c r="AC23" s="15"/>
     </row>
-    <row r="24" spans="6:29" s="6" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="24" spans="6:29" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F24" s="16"/>
       <c r="G24" s="16"/>
       <c r="J24" s="16"/>
       <c r="S24" s="16"/>
       <c r="T24" s="16"/>
     </row>
-    <row r="25" spans="6:29" s="6" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="25" spans="6:29" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F25" s="16"/>
       <c r="G25" s="16"/>
       <c r="J25" s="16"/>
       <c r="S25" s="16"/>
       <c r="T25" s="16"/>
     </row>
-    <row r="26" spans="6:29" s="6" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="26" spans="6:29" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F26" s="16"/>
       <c r="G26" s="16"/>
       <c r="J26" s="16"/>
       <c r="S26" s="16"/>
       <c r="T26" s="16"/>
     </row>
-    <row r="27" spans="6:29" s="15" customFormat="1" ht="43.45" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="27" spans="6:29" s="15" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F27" s="17"/>
       <c r="G27" s="17"/>
       <c r="J27" s="17"/>
@@ -4330,7 +4330,7 @@
       <c r="AB27" s="6"/>
       <c r="AC27" s="6"/>
     </row>
-    <row r="28" spans="6:29" s="15" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="28" spans="6:29" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F28" s="17"/>
       <c r="G28" s="17"/>
       <c r="J28" s="17"/>
@@ -4345,21 +4345,21 @@
       <c r="AB28" s="6"/>
       <c r="AC28" s="6"/>
     </row>
-    <row r="29" spans="6:29" s="6" customFormat="1" ht="43.45" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="29" spans="6:29" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F29" s="16"/>
       <c r="G29" s="16"/>
       <c r="J29" s="16"/>
       <c r="S29" s="16"/>
       <c r="T29" s="16"/>
     </row>
-    <row r="30" spans="6:29" s="6" customFormat="1" ht="43.45" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="30" spans="6:29" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F30" s="16"/>
       <c r="G30" s="16"/>
       <c r="J30" s="16"/>
       <c r="S30" s="16"/>
       <c r="T30" s="16"/>
     </row>
-    <row r="31" spans="6:29" s="6" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="31" spans="6:29" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F31" s="16"/>
       <c r="G31" s="16"/>
       <c r="J31" s="16"/>
@@ -4374,7 +4374,7 @@
       <c r="AB31" s="15"/>
       <c r="AC31" s="15"/>
     </row>
-    <row r="32" spans="6:29" s="6" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="32" spans="6:29" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F32" s="16"/>
       <c r="G32" s="16"/>
       <c r="J32" s="16"/>
@@ -4389,7 +4389,7 @@
       <c r="AB32" s="15"/>
       <c r="AC32" s="15"/>
     </row>
-    <row r="33" spans="6:29" s="6" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="33" spans="6:29" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F33" s="16"/>
       <c r="G33" s="16"/>
       <c r="J33" s="16"/>
@@ -4404,7 +4404,7 @@
       <c r="AB33" s="15"/>
       <c r="AC33" s="15"/>
     </row>
-    <row r="34" spans="6:29" s="6" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="34" spans="6:29" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F34" s="16"/>
       <c r="G34" s="16"/>
       <c r="J34" s="16"/>
@@ -4419,7 +4419,7 @@
       <c r="AB34" s="15"/>
       <c r="AC34" s="15"/>
     </row>
-    <row r="35" spans="6:29" s="15" customFormat="1" ht="43.45" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="35" spans="6:29" s="15" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F35" s="17"/>
       <c r="G35" s="17"/>
       <c r="J35" s="17"/>
@@ -4434,7 +4434,7 @@
       <c r="AB35" s="6"/>
       <c r="AC35" s="6"/>
     </row>
-    <row r="36" spans="6:29" s="15" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="36" spans="6:29" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F36" s="17"/>
       <c r="G36" s="17"/>
       <c r="J36" s="17"/>
@@ -4449,7 +4449,7 @@
       <c r="AB36" s="6"/>
       <c r="AC36" s="6"/>
     </row>
-    <row r="37" spans="6:29" s="15" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="37" spans="6:29" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F37" s="17"/>
       <c r="G37" s="17"/>
       <c r="J37" s="17"/>
@@ -4464,7 +4464,7 @@
       <c r="AB37" s="6"/>
       <c r="AC37" s="6"/>
     </row>
-    <row r="38" spans="6:29" s="6" customFormat="1" ht="43.45" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="38" spans="6:29" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F38" s="16"/>
       <c r="G38" s="16"/>
       <c r="J38" s="16"/>
@@ -4479,7 +4479,7 @@
       <c r="AB38" s="15"/>
       <c r="AC38" s="15"/>
     </row>
-    <row r="39" spans="6:29" s="6" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="39" spans="6:29" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F39" s="16"/>
       <c r="G39" s="16"/>
       <c r="J39" s="16"/>
@@ -4494,7 +4494,7 @@
       <c r="AB39" s="15"/>
       <c r="AC39" s="15"/>
     </row>
-    <row r="40" spans="6:29" x14ac:dyDescent="0.5">
+    <row r="40" spans="6:29" x14ac:dyDescent="0.25">
       <c r="V40" s="15"/>
       <c r="W40" s="15"/>
       <c r="X40" s="15"/>
@@ -4504,7 +4504,7 @@
       <c r="AB40" s="15"/>
       <c r="AC40" s="15"/>
     </row>
-    <row r="41" spans="6:29" x14ac:dyDescent="0.5">
+    <row r="41" spans="6:29" x14ac:dyDescent="0.25">
       <c r="V41" s="15"/>
       <c r="W41" s="15"/>
       <c r="X41" s="15"/>
@@ -4514,7 +4514,7 @@
       <c r="AB41" s="15"/>
       <c r="AC41" s="15"/>
     </row>
-    <row r="42" spans="6:29" x14ac:dyDescent="0.5">
+    <row r="42" spans="6:29" x14ac:dyDescent="0.25">
       <c r="V42" s="15"/>
       <c r="W42" s="15"/>
       <c r="X42" s="15"/>
@@ -4524,7 +4524,7 @@
       <c r="AB42" s="15"/>
       <c r="AC42" s="15"/>
     </row>
-    <row r="43" spans="6:29" x14ac:dyDescent="0.5">
+    <row r="43" spans="6:29" x14ac:dyDescent="0.25">
       <c r="V43" s="15"/>
       <c r="W43" s="15"/>
       <c r="X43" s="15"/>
@@ -4534,7 +4534,7 @@
       <c r="AB43" s="15"/>
       <c r="AC43" s="15"/>
     </row>
-    <row r="44" spans="6:29" x14ac:dyDescent="0.5">
+    <row r="44" spans="6:29" x14ac:dyDescent="0.25">
       <c r="V44" s="15"/>
       <c r="W44" s="15"/>
       <c r="X44" s="15"/>
@@ -4544,7 +4544,7 @@
       <c r="AB44" s="15"/>
       <c r="AC44" s="15"/>
     </row>
-    <row r="45" spans="6:29" x14ac:dyDescent="0.5">
+    <row r="45" spans="6:29" x14ac:dyDescent="0.25">
       <c r="V45" s="6"/>
       <c r="W45" s="6"/>
       <c r="X45" s="6"/>
@@ -4554,7 +4554,7 @@
       <c r="AB45" s="6"/>
       <c r="AC45" s="6"/>
     </row>
-    <row r="46" spans="6:29" x14ac:dyDescent="0.5">
+    <row r="46" spans="6:29" x14ac:dyDescent="0.25">
       <c r="V46" s="6"/>
       <c r="W46" s="6"/>
       <c r="X46" s="6"/>
@@ -4564,7 +4564,7 @@
       <c r="AB46" s="6"/>
       <c r="AC46" s="6"/>
     </row>
-    <row r="47" spans="6:29" x14ac:dyDescent="0.5">
+    <row r="47" spans="6:29" x14ac:dyDescent="0.25">
       <c r="V47" s="6"/>
       <c r="W47" s="6"/>
       <c r="X47" s="6"/>
@@ -4574,7 +4574,7 @@
       <c r="AB47" s="6"/>
       <c r="AC47" s="6"/>
     </row>
-    <row r="48" spans="6:29" x14ac:dyDescent="0.5">
+    <row r="48" spans="6:29" x14ac:dyDescent="0.25">
       <c r="V48" s="6"/>
       <c r="W48" s="6"/>
       <c r="X48" s="6"/>
@@ -4584,7 +4584,7 @@
       <c r="AB48" s="6"/>
       <c r="AC48" s="6"/>
     </row>
-    <row r="49" spans="22:29" x14ac:dyDescent="0.5">
+    <row r="49" spans="22:29" x14ac:dyDescent="0.25">
       <c r="V49" s="6"/>
       <c r="W49" s="6"/>
       <c r="X49" s="6"/>
@@ -4594,7 +4594,7 @@
       <c r="AB49" s="6"/>
       <c r="AC49" s="6"/>
     </row>
-    <row r="50" spans="22:29" x14ac:dyDescent="0.5">
+    <row r="50" spans="22:29" x14ac:dyDescent="0.25">
       <c r="V50" s="15"/>
       <c r="W50" s="15"/>
       <c r="X50" s="15"/>
@@ -4604,7 +4604,7 @@
       <c r="AB50" s="15"/>
       <c r="AC50" s="15"/>
     </row>
-    <row r="51" spans="22:29" x14ac:dyDescent="0.5">
+    <row r="51" spans="22:29" x14ac:dyDescent="0.25">
       <c r="V51" s="15"/>
       <c r="W51" s="15"/>
       <c r="X51" s="15"/>
@@ -4614,7 +4614,7 @@
       <c r="AB51" s="15"/>
       <c r="AC51" s="15"/>
     </row>
-    <row r="52" spans="22:29" x14ac:dyDescent="0.5">
+    <row r="52" spans="22:29" x14ac:dyDescent="0.25">
       <c r="V52" s="15"/>
       <c r="W52" s="15"/>
       <c r="X52" s="15"/>
@@ -4624,7 +4624,7 @@
       <c r="AB52" s="15"/>
       <c r="AC52" s="15"/>
     </row>
-    <row r="53" spans="22:29" x14ac:dyDescent="0.5">
+    <row r="53" spans="22:29" x14ac:dyDescent="0.25">
       <c r="V53" s="15"/>
       <c r="W53" s="15"/>
       <c r="X53" s="15"/>
@@ -4634,7 +4634,7 @@
       <c r="AB53" s="15"/>
       <c r="AC53" s="15"/>
     </row>
-    <row r="54" spans="22:29" x14ac:dyDescent="0.5">
+    <row r="54" spans="22:29" x14ac:dyDescent="0.25">
       <c r="V54" s="15"/>
       <c r="W54" s="15"/>
       <c r="X54" s="15"/>
@@ -4659,14 +4659,14 @@
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.29296875" customWidth="1"/>
-    <col min="2" max="2" width="27.87890625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.05859375" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -4677,7 +4677,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -4688,7 +4688,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -4699,7 +4699,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -4710,7 +4710,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -4721,7 +4721,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -4732,7 +4732,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -4743,7 +4743,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -4754,7 +4754,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -4765,7 +4765,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -4776,7 +4776,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -4787,7 +4787,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>49</v>
       </c>
@@ -4798,7 +4798,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>49</v>
       </c>
@@ -4809,7 +4809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -4820,7 +4820,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>1</v>
       </c>
@@ -4831,7 +4831,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -4842,7 +4842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -4867,15 +4867,15 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.17578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.8203125" customWidth="1"/>
-    <col min="3" max="3" width="14.17578125" customWidth="1"/>
-    <col min="4" max="4" width="27.05859375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -4889,7 +4889,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -4903,7 +4903,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -4917,7 +4917,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -4931,7 +4931,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -4945,7 +4945,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -4959,7 +4959,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -4973,7 +4973,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>41</v>
       </c>
@@ -4987,7 +4987,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>49</v>
       </c>
@@ -5001,7 +5001,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -5247,6 +5247,14 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Description0 xmlns="3dc215b4-4765-4137-95ef-e24fb8216673">Data and Metadata documentation will explain structure and content any QC manipulations that have been done to the data.</Description0>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -5255,22 +5263,39 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Description0 xmlns="3dc215b4-4765-4137-95ef-e24fb8216673">Data and Metadata documentation will explain structure and content any QC manipulations that have been done to the data.</Description0>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{914015FE-AEFC-40B4-9F7F-DA575E593C8A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{914015FE-AEFC-40B4-9F7F-DA575E593C8A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3dc215b4-4765-4137-95ef-e24fb8216673"/>
+    <ds:schemaRef ds:uri="2634c873-c79e-4fdd-b8bf-a33e5fa5c27f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{934B9C5C-492E-4847-8B6C-70ABA3C0C6BB}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{490A8145-0457-4251-A609-6BAF8EE09F01}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3dc215b4-4765-4137-95ef-e24fb8216673"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{490A8145-0457-4251-A609-6BAF8EE09F01}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{934B9C5C-492E-4847-8B6C-70ABA3C0C6BB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>